<commit_message>
pulling demographic information out
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -4,9 +4,9 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97441056-4218-A64B-9A10-3F0D4A6DFB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67D676F-AAAE-8443-9E41-8A883B038C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="1280" windowWidth="22240" windowHeight="15060" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="500" windowWidth="27580" windowHeight="17500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions for Use" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2136" uniqueCount="163">
   <si>
     <t>Date of Birth</t>
   </si>
@@ -558,6 +558,33 @@
   </si>
   <si>
     <t>Specify Date of Data Points Being Used</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Black/African/Caribbean/Black British</t>
+  </si>
+  <si>
+    <t>Neurodivergence (e.g. ASD or ADHD)</t>
+  </si>
+  <si>
+    <t>SGO</t>
+  </si>
+  <si>
+    <t>CCPT</t>
+  </si>
+  <si>
+    <t>Incarceration of a household member</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Prefer Not to Say</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1244,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1257,6 +1283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -18117,138 +18144,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="55" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="61">
+      <c r="A2" s="60">
         <f>'Goal Based Outcomes (GBO)'!C7</f>
         <v>1</v>
       </c>
-      <c r="B2" s="54">
+      <c r="B2" s="53">
         <f>'Goal Based Outcomes (GBO)'!D2</f>
         <v>0</v>
       </c>
-      <c r="C2" s="54">
+      <c r="C2" s="53">
         <f>'Goal Based Outcomes (GBO)'!D7</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="61">
+      <c r="A3" s="60">
         <f>'Goal Based Outcomes (GBO)'!C8</f>
         <v>2</v>
       </c>
-      <c r="B3" s="54">
+      <c r="B3" s="53">
         <f>'Goal Based Outcomes (GBO)'!D2</f>
         <v>0</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="53">
         <f>'Goal Based Outcomes (GBO)'!D8</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="61">
+      <c r="A4" s="60">
         <f>'Goal Based Outcomes (GBO)'!C9</f>
         <v>3</v>
       </c>
-      <c r="B4" s="54">
+      <c r="B4" s="53">
         <f>'Goal Based Outcomes (GBO)'!D2</f>
         <v>0</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="53">
         <f>'Goal Based Outcomes (GBO)'!D9</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="61">
+      <c r="A5" s="60">
         <f>'Goal Based Outcomes (GBO)'!C10</f>
         <v>4</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="53">
         <f>'Goal Based Outcomes (GBO)'!D2</f>
         <v>0</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="53">
         <f>'Goal Based Outcomes (GBO)'!D10</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="61">
+      <c r="A6" s="60">
         <f>'Goal Based Outcomes (GBO)'!C11</f>
         <v>5</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="53">
         <f>'Goal Based Outcomes (GBO)'!D2</f>
         <v>0</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="53">
         <f>'Goal Based Outcomes (GBO)'!D11</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="61">
+      <c r="A7" s="60">
         <f>'Goal Based Outcomes (GBO)'!C12</f>
         <v>6</v>
       </c>
-      <c r="B7" s="54">
+      <c r="B7" s="53">
         <f>'Goal Based Outcomes (GBO)'!D2</f>
         <v>0</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="53">
         <f>'Goal Based Outcomes (GBO)'!D12</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="61">
+      <c r="A8" s="60">
         <f>'Goal Based Outcomes (GBO)'!C13</f>
         <v>7</v>
       </c>
-      <c r="B8" s="54">
+      <c r="B8" s="53">
         <f>'Goal Based Outcomes (GBO)'!D2</f>
         <v>0</v>
       </c>
-      <c r="C8" s="54">
+      <c r="C8" s="53">
         <f>'Goal Based Outcomes (GBO)'!D13</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="61">
+      <c r="A9" s="60">
         <f>'Goal Based Outcomes (GBO)'!C14</f>
         <v>8</v>
       </c>
-      <c r="B9" s="54">
+      <c r="B9" s="53">
         <f>'Goal Based Outcomes (GBO)'!D2</f>
         <v>0</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="53">
         <f>'Goal Based Outcomes (GBO)'!D14</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="61">
+      <c r="A10" s="60">
         <f>'Goal Based Outcomes (GBO)'!C15</f>
         <v>9</v>
       </c>
-      <c r="B10" s="54">
+      <c r="B10" s="53">
         <f>'Goal Based Outcomes (GBO)'!D10</f>
         <v>0</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="53">
         <f>'Goal Based Outcomes (GBO)'!D15</f>
         <v>0</v>
       </c>
@@ -18282,52 +18309,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="14" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="55" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="58" t="s">
+      <c r="K1" s="57" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="55"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
@@ -18459,36 +18486,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="14" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="57" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
@@ -18509,13 +18536,13 @@
       <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="34"/>
@@ -18536,13 +18563,13 @@
       <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="54"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="34"/>
@@ -18706,10 +18733,10 @@
     </row>
     <row r="14" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17"/>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="59" t="s">
+      <c r="F14" s="58" t="s">
         <v>102</v>
       </c>
       <c r="G14" s="14"/>
@@ -18723,16 +18750,16 @@
     </row>
     <row r="15" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
-      <c r="C15" s="70" t="s">
+      <c r="C15" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="67" t="s">
+      <c r="D15" s="66" t="s">
         <v>153</v>
       </c>
-      <c r="E15" s="66" t="s">
+      <c r="E15" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="F15" s="59" t="s">
+      <c r="F15" s="58" t="s">
         <v>144</v>
       </c>
       <c r="H15" s="21" t="s">
@@ -18751,14 +18778,14 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="17"/>
-      <c r="C16" s="71" t="s">
+      <c r="C16" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="73">
+      <c r="D16" s="72">
         <v>45382</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="60"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="59"/>
       <c r="H16" s="25"/>
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
@@ -18767,13 +18794,13 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="17"/>
-      <c r="C17" s="71" t="s">
+      <c r="C17" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="74">
+      <c r="D17" s="73">
         <v>45473</v>
       </c>
-      <c r="E17" s="64"/>
+      <c r="E17" s="63"/>
       <c r="F17" s="31"/>
       <c r="H17" s="25"/>
       <c r="I17" s="26"/>
@@ -18783,13 +18810,13 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="17"/>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="74">
+      <c r="D18" s="73">
         <v>45565</v>
       </c>
-      <c r="E18" s="64"/>
+      <c r="E18" s="63"/>
       <c r="F18" s="31"/>
       <c r="H18" s="25"/>
       <c r="I18" s="26"/>
@@ -18799,11 +18826,11 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="17"/>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="68"/>
-      <c r="E19" s="64"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="63"/>
       <c r="F19" s="31"/>
       <c r="H19" s="25"/>
       <c r="I19" s="26"/>
@@ -18813,11 +18840,11 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="17"/>
-      <c r="C20" s="71" t="s">
+      <c r="C20" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="68"/>
-      <c r="E20" s="64"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="63"/>
       <c r="F20" s="31"/>
       <c r="H20" s="25"/>
       <c r="I20" s="26"/>
@@ -18827,11 +18854,11 @@
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="17"/>
-      <c r="C21" s="71" t="s">
+      <c r="C21" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="68"/>
-      <c r="E21" s="64"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="63"/>
       <c r="F21" s="31"/>
       <c r="H21" s="25"/>
       <c r="I21" s="26"/>
@@ -18841,11 +18868,11 @@
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="17"/>
-      <c r="C22" s="71" t="s">
+      <c r="C22" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="68"/>
-      <c r="E22" s="64"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="63"/>
       <c r="F22" s="31"/>
       <c r="H22" s="25"/>
       <c r="I22" s="26"/>
@@ -18855,11 +18882,11 @@
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="17"/>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="68"/>
-      <c r="E23" s="64"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="63"/>
       <c r="F23" s="31"/>
       <c r="H23" s="25"/>
       <c r="I23" s="26"/>
@@ -18869,11 +18896,11 @@
     </row>
     <row r="24" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
-      <c r="C24" s="72" t="s">
+      <c r="C24" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="69"/>
-      <c r="E24" s="65"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="64"/>
       <c r="F24" s="32"/>
       <c r="H24" s="28"/>
       <c r="I24" s="29"/>
@@ -19036,8 +19063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19086,16 +19113,36 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="50"/>
+      <c r="A2" s="74">
+        <v>30437</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="J2" s="49" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C3" s="15"/>
@@ -19121,7 +19168,7 @@
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
-      <c r="F6" s="62"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
@@ -19616,7 +19663,7 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="51"/>
+      <c r="D7" s="50"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
@@ -19625,7 +19672,7 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" s="52"/>
+      <c r="D8" s="51"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
@@ -19634,7 +19681,7 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="52"/>
+      <c r="D9" s="51"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
@@ -19643,7 +19690,7 @@
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="D10" s="52"/>
+      <c r="D10" s="51"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
@@ -19652,7 +19699,7 @@
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="D11" s="52"/>
+      <c r="D11" s="51"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
@@ -19661,7 +19708,7 @@
       <c r="C12">
         <v>6</v>
       </c>
-      <c r="D12" s="52"/>
+      <c r="D12" s="51"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
@@ -19670,7 +19717,7 @@
       <c r="C13">
         <v>7</v>
       </c>
-      <c r="D13" s="52"/>
+      <c r="D13" s="51"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
@@ -19679,7 +19726,7 @@
       <c r="C14">
         <v>8</v>
       </c>
-      <c r="D14" s="52"/>
+      <c r="D14" s="51"/>
     </row>
     <row r="15" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -19688,7 +19735,7 @@
       <c r="C15">
         <v>9</v>
       </c>
-      <c r="D15" s="53"/>
+      <c r="D15" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -19714,7 +19761,7 @@
   <dimension ref="C1:Q95"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21117,8 +21164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92C8DBC-9A58-4D37-8A6A-DC4C3684B531}">
   <dimension ref="C1:Q95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>